<commit_message>
Correction lsite distribution des cartes
</commit_message>
<xml_diff>
--- a/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
+++ b/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmorelle\Documents\Thèse\Expériences\Expé 2\PFE_DEBIDOUR_DELLA-NEGRA\Dossier de rendu phase B\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913E63FC-60E0-40EF-9692-DD5C0DD2F4D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="42" windowWidth="15960" windowHeight="18078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Liste tour par tour de distribu" sheetId="1" r:id="rId4"/>
+    <sheet name="Liste tour par tour de distribu" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Exemple d’une liste tour par tour de distribution des cartes</t>
   </si>
@@ -67,9 +76,6 @@
     <t>Conque</t>
   </si>
   <si>
-    <t>Hâche</t>
-  </si>
-  <si>
     <t>Distribution tour 2</t>
   </si>
   <si>
@@ -79,9 +85,6 @@
     <t>Ticket de lotterie gagnant</t>
   </si>
   <si>
-    <t>Jeux de société Quoridor</t>
-  </si>
-  <si>
     <t>Distribution tour 3</t>
   </si>
   <si>
@@ -122,15 +125,24 @@
   </si>
   <si>
     <t>Poisson pourri</t>
+  </si>
+  <si>
+    <t>Hache</t>
+  </si>
+  <si>
+    <t>Jeu de société Quoridor</t>
+  </si>
+  <si>
+    <t>Taser</t>
+  </si>
+  <si>
+    <t>Magazine minceur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -143,7 +155,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -169,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -282,48 +294,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -333,26 +361,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -551,7 +638,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -569,7 +656,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -598,7 +685,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -623,7 +710,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -648,7 +735,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -673,7 +760,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -698,7 +785,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -723,7 +810,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -748,7 +835,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -773,7 +860,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -798,7 +885,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -811,9 +898,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -830,7 +923,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -848,7 +941,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -873,7 +966,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -898,7 +991,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -923,7 +1016,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -948,7 +1041,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -973,7 +1066,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -998,7 +1091,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1023,7 +1116,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1048,7 +1141,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1073,7 +1166,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1086,9 +1179,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1102,7 +1201,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1120,7 +1219,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,7 +1248,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1174,7 +1273,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +1298,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1224,7 +1323,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1249,7 +1348,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1274,7 +1373,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1299,7 +1398,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1324,7 +1423,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1349,7 +1448,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1362,233 +1461,243 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="6" width="16.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="27.7" customHeight="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
+    <row r="2" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+    <row r="3" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" t="s" s="9">
+    <row r="4" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.05" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="10">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s" s="10">
+      <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" t="s" s="9">
+    <row r="6" spans="1:5" ht="32.049999999999997" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="10">
+      <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="10">
+      <c r="E6" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s" s="10">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s" s="10">
-        <v>13</v>
+    <row r="7" spans="1:5" ht="20.05" customHeight="1">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s" s="10">
+    <row r="8" spans="1:5" ht="32.049999999999997" customHeight="1">
+      <c r="A8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s" s="10">
-        <v>18</v>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="8" ht="32.05" customHeight="1">
-      <c r="A8" t="s" s="11">
+    <row r="9" spans="1:5" ht="20.05" customHeight="1">
+      <c r="A9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.05" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="32.049999999999997" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s" s="10">
+      <c r="C11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20.05" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="32.049999999999997" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s" s="10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="11">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s" s="9">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s" s="10">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s" s="10">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="11">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="10">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s" s="10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" ht="32.05" customHeight="1">
-      <c r="A11" t="s" s="11">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s" s="10">
+      <c r="D13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="11">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" ht="32.05" customHeight="1">
-      <c r="A13" t="s" s="11">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s" s="9">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s" s="10">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1596,8 +1705,8 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:A6"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Réorganisation dossier (changement de l'ordre des questionnaires)
</commit_message>
<xml_diff>
--- a/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
+++ b/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmorelle\Documents\Thèse\Expériences\Expé 2\PFE_DEBIDOUR_DELLA-NEGRA\Dossier de rendu phase B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913E63FC-60E0-40EF-9692-DD5C0DD2F4D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1842F7AF-A9D5-48E5-8A3F-DD85DAB448B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="42" windowWidth="15960" windowHeight="18078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
-    <t>Exemple d’une liste tour par tour de distribution des cartes</t>
-  </si>
-  <si>
     <t>Joueur 1</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>Magazine minceur</t>
+  </si>
+  <si>
+    <t>Liste tour par tour de distribution des cartes</t>
   </si>
 </sst>
 </file>
@@ -347,11 +347,11 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1486,7 +1486,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1497,7 +1497,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="27.7" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1507,197 +1507,197 @@
     <row r="2" spans="1:5" ht="20.25" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20.25" customHeight="1">
       <c r="A3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A4" s="12"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.05" customHeight="1">
       <c r="A7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32.049999999999997" customHeight="1">
       <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.05" customHeight="1">
       <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.05" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="32.049999999999997" customHeight="1">
       <c r="A11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.05" customHeight="1">
       <c r="A12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="32.049999999999997" customHeight="1">
       <c r="A13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour protocole & correction schémas
</commit_message>
<xml_diff>
--- a/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
+++ b/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmorelle\Documents\Thèse\Expériences\Expé 2\PFE_DEBIDOUR_DELLA-NEGRA\Dossier de rendu phase B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125805F-7853-4474-BE9A-AE65A9585C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE653C02-0292-4FD9-9960-8CF6B633F054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="42" windowWidth="15960" windowHeight="18078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -323,9 +323,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -338,9 +335,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -350,8 +344,14 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1486,7 +1486,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1496,207 +1496,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.7" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:5" ht="31.5" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Quelques corrections protocole + ajout questionnaire GMDS dans le protocole
</commit_message>
<xml_diff>
--- a/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
+++ b/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmorelle\Documents\Thèse\Expériences\Expé 2\PFE_DEBIDOUR_DELLA-NEGRA\Dossier de rendu phase B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE653C02-0292-4FD9-9960-8CF6B633F054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DF157E-400C-41D9-9512-2779F933A350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="42" windowWidth="15960" windowHeight="18078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Joueur 1</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Clé de voiture</t>
   </si>
   <si>
-    <t>Ticket de lotterie gagnant</t>
-  </si>
-  <si>
     <t>Distribution tour 3</t>
   </si>
   <si>
@@ -137,6 +134,12 @@
   </si>
   <si>
     <t>Nouilles chinoises</t>
+  </si>
+  <si>
+    <t>Ticket de loterie gagnant</t>
+  </si>
+  <si>
+    <t>Clé de voiture de luxe</t>
   </si>
 </sst>
 </file>
@@ -335,6 +338,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -344,13 +353,7 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1486,7 +1489,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1496,31 +1499,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.7" customHeight="1">
-      <c r="A1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1537,7 +1540,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A4" s="9"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1552,7 +1555,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1567,7 +1570,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1578,28 +1581,28 @@
         <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1612,92 +1615,92 @@
         <v>15</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A10" s="12" t="s">
-        <v>23</v>
+      <c r="A10" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.05" customHeight="1">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="32.049999999999997" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>30</v>
+      <c r="A13" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalisation doc fil d'ariane
</commit_message>
<xml_diff>
--- a/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
+++ b/Dossier de rendu phase B/Liste tour par tour de distribution des cartes - PFE Galèrapagos V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmorelle\Documents\Thèse\Expériences\Expé 2\PFE_DEBIDOUR_DELLA-NEGRA\Dossier de rendu phase B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DF157E-400C-41D9-9512-2779F933A350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190421FB-F987-49FB-A7F8-90AC36F2BAA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="42" windowWidth="15960" windowHeight="18078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Joueur 1</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Clé de voiture de luxe</t>
+  </si>
+  <si>
+    <t>Brosse à WC</t>
   </si>
 </sst>
 </file>
@@ -1489,7 +1492,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1643,7 +1646,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>14</v>
@@ -1677,7 +1680,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>7</v>
@@ -1700,7 +1703,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>